<commit_message>
Running the simulations with updated IBF and recording the results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IBF Decoding" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>10K</t>
   </si>
@@ -69,12 +69,6 @@
     <t>4 HashCount</t>
   </si>
   <si>
-    <t>HAD THROW EXCEPTION TURNED ON</t>
-  </si>
-  <si>
-    <t>HAD THROW EXCEPTION TURNED OFF</t>
-  </si>
-  <si>
     <t xml:space="preserve">In the original paper, the scaling overhead drops sharply as the number of cells per IBF is increased from 10 to 40, and reaches a point of diminishing returns after 80 cells. With 80 cells per strata, any estimate returned by the Strata Estimator should be scaled by a factor of 1.39 (in our case 2.10) to ensure that it will be greater than or equal to d 99% of th time. </t>
   </si>
   <si>
@@ -91,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Overhead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -198,8 +195,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -245,7 +262,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,13 +281,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -291,6 +310,16 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -310,6 +339,16 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,34 +468,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9560001</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95900035</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9480002</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9449999</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9435995</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92433363</c:v>
+                  <c:v>0.972333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8157141</c:v>
+                  <c:v>0.702857142857143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40299997</c:v>
+                  <c:v>0.2775</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1675556</c:v>
+                  <c:v>0.120888888888888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.08999996</c:v>
+                  <c:v>0.0727999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,34 +568,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9760001</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95900035</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9500002</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93950003</c:v>
+                  <c:v>0.998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93199944</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92533374</c:v>
+                  <c:v>0.978333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81999993</c:v>
+                  <c:v>0.661142857142857</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.41875008</c:v>
+                  <c:v>0.246499999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19622219</c:v>
+                  <c:v>0.135999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.09539999</c:v>
+                  <c:v>0.0738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -629,84 +668,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94200003</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9640002</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95200026</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93899965</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94639945</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92066705</c:v>
+                  <c:v>0.961666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77199996</c:v>
+                  <c:v>0.740571428571428</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40075</c:v>
+                  <c:v>0.245749999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18666668</c:v>
+                  <c:v>0.132666666666666</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10119998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>100K</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'IBF Decoding'!$E$6:$E$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.9620001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9430003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.94533366</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.94899976</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9455994</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.93533355</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.79571414</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.4337499</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.16688885</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.097999945</c:v>
+                  <c:v>0.0796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,11 +710,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="2125510280"/>
-        <c:axId val="2125503176"/>
+        <c:axId val="2060985432"/>
+        <c:axId val="2060992472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2125510280"/>
+        <c:axId val="2060985432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +747,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125503176"/>
+        <c:crossAx val="2060992472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -766,7 +755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125503176"/>
+        <c:axId val="2060992472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,7 +785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125510280"/>
+        <c:crossAx val="2060985432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -931,34 +920,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.975399999999998</c:v>
+                  <c:v>0.9954</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.971299999999996</c:v>
+                  <c:v>0.984099999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.959599999999995</c:v>
+                  <c:v>0.975533333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.949200000000002</c:v>
+                  <c:v>0.957249999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.909319999999999</c:v>
+                  <c:v>0.921439999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.840766666666664</c:v>
+                  <c:v>0.84693333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.749428571428568</c:v>
+                  <c:v>0.73905714285714</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.611699999999999</c:v>
+                  <c:v>0.5922</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.483799999999999</c:v>
+                  <c:v>0.450977777777778</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.376699999999999</c:v>
+                  <c:v>0.349179999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1034,34 +1023,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9972</c:v>
+                  <c:v>0.9996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.994399999999999</c:v>
+                  <c:v>0.9994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.990533333333333</c:v>
+                  <c:v>0.998933333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.983799999999998</c:v>
+                  <c:v>0.997949999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.975199999999996</c:v>
+                  <c:v>0.992759999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.960733333333328</c:v>
+                  <c:v>0.980566666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.893571428571429</c:v>
+                  <c:v>0.886114285714285</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.64485</c:v>
+                  <c:v>0.56495</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.370333333333334</c:v>
+                  <c:v>0.294177777777778</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.223899999999999</c:v>
+                  <c:v>0.187199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,34 +1126,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.957399999999997</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.954199999999994</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95006666666666</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.949300000000003</c:v>
+                  <c:v>0.99985</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.937679999999999</c:v>
+                  <c:v>0.99848</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.925399999999995</c:v>
+                  <c:v>0.978899999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.812685714285712</c:v>
+                  <c:v>0.700857142857144</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.411599999999999</c:v>
+                  <c:v>0.259099999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.181244444444445</c:v>
+                  <c:v>0.125466666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10032</c:v>
+                  <c:v>0.0736800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,34 +1229,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9956</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.990599999999999</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.978666666666667</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.974449999999996</c:v>
+                  <c:v>0.9999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.965279999999994</c:v>
+                  <c:v>0.99848</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.892333333333327</c:v>
+                  <c:v>0.823699999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.456171428571428</c:v>
+                  <c:v>0.262628571428572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.149575</c:v>
+                  <c:v>0.0993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0707555555555564</c:v>
+                  <c:v>0.0512222222222226</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0373799999999997</c:v>
+                  <c:v>0.0274799999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1343,34 +1332,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.976999999999999</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.974699999999997</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.968733333333328</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.966600000000002</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.946359999999999</c:v>
+                  <c:v>0.94768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.668799999999998</c:v>
+                  <c:v>0.392133333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2086</c:v>
+                  <c:v>0.0985142857142865</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.073925</c:v>
+                  <c:v>0.0435499999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0339333333333333</c:v>
+                  <c:v>0.0203999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0171799999999998</c:v>
+                  <c:v>0.0111399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,11 +1376,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127774136"/>
-        <c:axId val="2127779832"/>
+        <c:axId val="2043423624"/>
+        <c:axId val="2043429320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127774136"/>
+        <c:axId val="2043423624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1409,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127779832"/>
+        <c:crossAx val="2043429320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127779832"/>
+        <c:axId val="2043429320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1463,7 +1452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127774136"/>
+        <c:crossAx val="2043423624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1607,49 +1596,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.25833335518836</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1708333492279</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.07976192235946</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0347222328186</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0361111164093</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0333333492279</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0472222328186</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1208333492279</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.01666667461395</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0222222328186</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0236111164093</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.01805555820465</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.01666667461395</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0125</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0222222328186</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,49 +1723,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.35302535295486</c:v>
+                  <c:v>1.07529926896095</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.19337387681007</c:v>
+                  <c:v>1.08812698423862</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.12745447754859</c:v>
+                  <c:v>1.01024079322814</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.09899389147758</c:v>
+                  <c:v>1.01242186427116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.10483686327934</c:v>
+                  <c:v>1.01861750781536</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.07639843821525</c:v>
+                  <c:v>1.04172211289405</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.07104567289352</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0706492125988</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.78515860438346</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.59353239536285</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.57290036082267</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.07254037857055</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.32256779670715</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.15959200859069</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.30143299102783</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1861,49 +1850,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.60872658491134</c:v>
+                  <c:v>1.0741450458765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.34214479923248</c:v>
+                  <c:v>1.15862672030925</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.29493755698204</c:v>
+                  <c:v>1.0487130254507</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.19441853165626</c:v>
+                  <c:v>1.07029258310794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.29562551379203</c:v>
+                  <c:v>1.02535218298435</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.13512542247772</c:v>
+                  <c:v>1.03294682800769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.15667406916618</c:v>
+                  <c:v>1.04675229787826</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.15985943078994</c:v>
+                  <c:v>1.03276591300964</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.14453493952751</c:v>
+                  <c:v>1.03747597336769</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.12665985822677</c:v>
+                  <c:v>1.02548971176147</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.08116503953933</c:v>
+                  <c:v>1.00244799256324</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.11044785380363</c:v>
+                  <c:v>1.00696150064468</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.067961114645</c:v>
+                  <c:v>1.02781194150447</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.08632844686508</c:v>
+                  <c:v>1.01527112722396</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.06947393417358</c:v>
+                  <c:v>1.03154512643814</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,49 +1977,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.98779646158218</c:v>
+                  <c:v>1.2318112373352</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.44240890741348</c:v>
+                  <c:v>1.15470606386661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.67461513280868</c:v>
+                  <c:v>1.17617998421192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.34885258078575</c:v>
+                  <c:v>1.14235059022903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.25737380385398</c:v>
+                  <c:v>1.03542059063911</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.20152360796928</c:v>
+                  <c:v>1.03215854465961</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.19653933644294</c:v>
+                  <c:v>1.05046499371528</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.19266700744628</c:v>
+                  <c:v>1.10436962544918</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.18802984952926</c:v>
+                  <c:v>1.10242941081523</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.16845017671585</c:v>
+                  <c:v>1.08398702144622</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.17634398937225</c:v>
+                  <c:v>1.07758920788764</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.10716916322708</c:v>
+                  <c:v>1.06128992140293</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.07735979557037</c:v>
+                  <c:v>1.04403171837329</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.12588908672332</c:v>
+                  <c:v>1.06155008971691</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.06585914492607</c:v>
+                  <c:v>1.04729796051979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2047,11 +2036,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127831096"/>
-        <c:axId val="2127836904"/>
+        <c:axId val="2043480456"/>
+        <c:axId val="2043486264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127831096"/>
+        <c:axId val="2043480456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2085,7 +2074,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127836904"/>
+        <c:crossAx val="2043486264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2093,7 +2082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127836904"/>
+        <c:axId val="2043486264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127831096"/>
+        <c:crossAx val="2043480456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8205,11 +8194,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2131272040"/>
-        <c:axId val="2131286264"/>
+        <c:axId val="2043358472"/>
+        <c:axId val="2043454152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2131272040"/>
+        <c:axId val="2043358472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8219,7 +8208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131286264"/>
+        <c:crossAx val="2043454152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8227,7 +8216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131286264"/>
+        <c:axId val="2043454152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8238,7 +8227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131272040"/>
+        <c:crossAx val="2043358472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8265,15 +8254,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:colOff>101600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8725,7 +8714,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8744,209 +8733,177 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5">
         <v>100</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>0</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.95600010000000002</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.97600010000000004</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.94200002999999999</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.96200010000000002</v>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>0.95900034999999995</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.95900034999999995</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.96400019999999997</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.94300030000000001</v>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>15</v>
       </c>
-      <c r="B9" s="1">
-        <v>0.94800019999999996</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.95000019999999996</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.95200026000000004</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.94533365999999996</v>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>20</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.9449999</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.93950003000000004</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.93899964999999996</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.94899975999999997</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.998</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>25</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.94359950000000004</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.93199944000000001</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.94639945000000003</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.94559939999999998</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>30</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.92433363000000002</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.92533374000000002</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.92066705000000004</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.93533354999999996</v>
+      <c r="B12">
+        <v>0.97233333333333305</v>
+      </c>
+      <c r="C12">
+        <v>0.97833333333333306</v>
+      </c>
+      <c r="D12">
+        <v>0.961666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>35</v>
       </c>
-      <c r="B13" s="1">
-        <v>0.8157141</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.81999993000000004</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.77199996000000004</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.79571413999999996</v>
+      <c r="B13">
+        <v>0.70285714285714296</v>
+      </c>
+      <c r="C13">
+        <v>0.66114285714285703</v>
+      </c>
+      <c r="D13">
+        <v>0.74057142857142799</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>40</v>
       </c>
-      <c r="B14" s="1">
-        <v>0.40299996999999999</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.41875008000000002</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.40075</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.43374990000000002</v>
+      <c r="B14">
+        <v>0.27750000000000002</v>
+      </c>
+      <c r="C14">
+        <v>0.246499999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.245749999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>45</v>
       </c>
-      <c r="B15" s="1">
-        <v>0.1675556</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.19622218999999999</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.18666668</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.16688885000000001</v>
+      <c r="B15">
+        <v>0.120888888888888</v>
+      </c>
+      <c r="C15">
+        <v>0.13599999999999901</v>
+      </c>
+      <c r="D15">
+        <v>0.13266666666666599</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>50</v>
       </c>
-      <c r="B16" s="1">
-        <v>8.9999960000000004E-2</v>
-      </c>
-      <c r="C16" s="3">
-        <v>9.5399990000000004E-2</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.10119997999999999</v>
-      </c>
-      <c r="E16" s="1">
-        <v>9.7999945000000005E-2</v>
+      <c r="B16">
+        <v>7.2799999999999906E-2</v>
+      </c>
+      <c r="C16">
+        <v>7.3800000000000004E-2</v>
+      </c>
+      <c r="D16">
+        <v>7.9600000000000004E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -8958,10 +8915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:F23"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8989,34 +8946,34 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="10">
         <v>1</v>
       </c>
       <c r="E5" s="1">
@@ -9027,325 +8984,357 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.97539999999999805</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.99719999999999998</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.95739999999999703</v>
+      <c r="B6" s="10">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>0.99560000000000004</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>0.97699999999999898</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.97129999999999606</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.99439999999999895</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.95419999999999405</v>
+      <c r="B7" s="10">
+        <v>0.98409999999999898</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.99939999999999996</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>0.99059999999999904</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>0.97469999999999701</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>0.95959999999999501</v>
+        <v>0.97553333333333303</v>
       </c>
       <c r="C8" s="1">
-        <v>0.99053333333333304</v>
+        <v>0.99893333333333301</v>
       </c>
       <c r="D8" s="1">
-        <v>0.95006666666665995</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>0.97866666666666702</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>0.96873333333332801</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>0.94920000000000204</v>
+        <v>0.95724999999999705</v>
       </c>
       <c r="C9" s="1">
-        <v>0.98379999999999801</v>
+        <v>0.997949999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>0.94930000000000303</v>
+        <v>0.99985000000000002</v>
       </c>
       <c r="E9" s="1">
-        <v>0.97444999999999604</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="F9" s="1">
-        <v>0.96660000000000201</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>25</v>
       </c>
       <c r="B10" s="1">
-        <v>0.90931999999999902</v>
+        <v>0.92143999999999604</v>
       </c>
       <c r="C10" s="1">
-        <v>0.97519999999999596</v>
+        <v>0.99275999999999898</v>
       </c>
       <c r="D10" s="1">
-        <v>0.93767999999999896</v>
+        <v>0.99848000000000003</v>
       </c>
       <c r="E10" s="1">
-        <v>0.96527999999999403</v>
+        <v>0.99848000000000003</v>
       </c>
       <c r="F10" s="1">
-        <v>0.94635999999999898</v>
+        <v>0.94767999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>30</v>
       </c>
       <c r="B11" s="1">
-        <v>0.840766666666664</v>
+        <v>0.84693333333332999</v>
       </c>
       <c r="C11" s="1">
-        <v>0.960733333333328</v>
+        <v>0.98056666666666603</v>
       </c>
       <c r="D11" s="1">
-        <v>0.925399999999995</v>
+        <v>0.97889999999999899</v>
       </c>
       <c r="E11" s="1">
-        <v>0.89233333333332698</v>
+        <v>0.82369999999999899</v>
       </c>
       <c r="F11" s="1">
-        <v>0.66879999999999795</v>
+        <v>0.392133333333334</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>0.749428571428568</v>
+        <v>0.73905714285713997</v>
       </c>
       <c r="C12" s="1">
-        <v>0.89357142857142902</v>
+        <v>0.88611428571428497</v>
       </c>
       <c r="D12" s="1">
-        <v>0.81268571428571201</v>
+        <v>0.70085714285714396</v>
       </c>
       <c r="E12" s="1">
-        <v>0.45617142857142801</v>
+        <v>0.26262857142857199</v>
       </c>
       <c r="F12" s="1">
-        <v>0.20860000000000001</v>
+        <v>9.8514285714286498E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>40</v>
       </c>
       <c r="B13" s="1">
-        <v>0.61169999999999902</v>
+        <v>0.59219999999999995</v>
       </c>
       <c r="C13" s="1">
-        <v>0.64485000000000003</v>
+        <v>0.56494999999999995</v>
       </c>
       <c r="D13" s="1">
-        <v>0.41159999999999902</v>
+        <v>0.259099999999999</v>
       </c>
       <c r="E13" s="1">
-        <v>0.14957500000000001</v>
+        <v>9.9299999999999999E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>7.3925000000000005E-2</v>
+        <v>4.35499999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>45</v>
       </c>
       <c r="B14" s="1">
-        <v>0.48379999999999901</v>
+        <v>0.45097777777777798</v>
       </c>
       <c r="C14" s="1">
-        <v>0.37033333333333401</v>
+        <v>0.29417777777777798</v>
       </c>
       <c r="D14" s="1">
-        <v>0.18124444444444501</v>
+        <v>0.125466666666667</v>
       </c>
       <c r="E14" s="1">
-        <v>7.0755555555556404E-2</v>
+        <v>5.1222222222222599E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>3.3933333333333301E-2</v>
+        <v>2.0399999999999901E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>50</v>
       </c>
       <c r="B15" s="1">
-        <v>0.37669999999999898</v>
+        <v>0.34917999999999899</v>
       </c>
       <c r="C15" s="1">
-        <v>0.22389999999999899</v>
+        <v>0.18719999999999901</v>
       </c>
       <c r="D15" s="1">
-        <v>0.10032000000000001</v>
+        <v>7.3680000000000107E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>3.7379999999999698E-2</v>
+        <v>2.7479999999999699E-2</v>
       </c>
       <c r="F15" s="1">
-        <v>1.71799999999998E-2</v>
+        <v>1.11399999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" ht="75" customHeight="1">
-      <c r="A27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A19:F23"/>
-    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -9359,8 +9348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9382,255 +9371,255 @@
       <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5">
         <v>20</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>30</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>40</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>50</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>60</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>70</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>80</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>90</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>100</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>110</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>120</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>130</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>140</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>150</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.25833335518836</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1.1708333492278999</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1.0797619223594599</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1.0347222328186001</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1.0361111164093</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1.0333333492279</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>1.0472222328186001</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1.1208333492278999</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>1.0166666746139501</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>1.0222222328185999</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>1.0236111164093</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>1.01805555820465</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>1.0166666746139501</v>
+        <v>1</v>
       </c>
       <c r="O5">
-        <v>1.0125</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>1.0222222328185999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>100</v>
       </c>
       <c r="B6">
-        <v>2.3530253529548601</v>
+        <v>1.07529926896095</v>
       </c>
       <c r="C6">
-        <v>2.1933738768100701</v>
+        <v>1.0881269842386201</v>
       </c>
       <c r="D6">
-        <v>2.1274544775485902</v>
+        <v>1.0102407932281401</v>
       </c>
       <c r="E6">
-        <v>2.0989938914775799</v>
+        <v>1.01242186427116</v>
       </c>
       <c r="F6">
-        <v>2.1048368632793402</v>
+        <v>1.0186175078153601</v>
       </c>
       <c r="G6">
-        <v>2.0763984382152501</v>
+        <v>1.0417221128940499</v>
       </c>
       <c r="H6">
-        <v>2.0710456728935198</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>2.0706492125987999</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>1.78515860438346</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>1.59353239536285</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1.5729003608226699</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1.0725403785705501</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>1.3225677967071501</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>1.1595920085906899</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>1.3014329910278299</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7">
-        <v>2.6087265849113401</v>
+        <v>1.0741450458765001</v>
       </c>
       <c r="C7">
-        <v>2.34214479923248</v>
+        <v>1.15862672030925</v>
       </c>
       <c r="D7">
-        <v>2.2949375569820401</v>
+        <v>1.0487130254507</v>
       </c>
       <c r="E7">
-        <v>2.1944185316562601</v>
+        <v>1.07029258310794</v>
       </c>
       <c r="F7">
-        <v>2.2956255137920301</v>
+        <v>1.0253521829843499</v>
       </c>
       <c r="G7">
-        <v>2.1351254224777199</v>
+        <v>1.0329468280076901</v>
       </c>
       <c r="H7">
-        <v>2.1566740691661801</v>
+        <v>1.04675229787826</v>
       </c>
       <c r="I7">
-        <v>2.1598594307899401</v>
+        <v>1.03276591300964</v>
       </c>
       <c r="J7">
-        <v>2.1445349395275102</v>
+        <v>1.0374759733676899</v>
       </c>
       <c r="K7">
-        <v>2.1266598582267702</v>
+        <v>1.0254897117614701</v>
       </c>
       <c r="L7">
-        <v>2.08116503953933</v>
+        <v>1.0024479925632399</v>
       </c>
       <c r="M7">
-        <v>2.1104478538036302</v>
+        <v>1.0069615006446799</v>
       </c>
       <c r="N7">
-        <v>2.0679611146450001</v>
+        <v>1.02781194150447</v>
       </c>
       <c r="O7">
-        <v>2.08632844686508</v>
+        <v>1.0152711272239601</v>
       </c>
       <c r="P7">
-        <v>2.0694739341735802</v>
+        <v>1.0315451264381399</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B8">
-        <v>2.9877964615821799</v>
+        <v>1.2318112373351999</v>
       </c>
       <c r="C8">
-        <v>2.4424089074134798</v>
+        <v>1.15470606386661</v>
       </c>
       <c r="D8">
-        <v>2.6746151328086798</v>
+        <v>1.17617998421192</v>
       </c>
       <c r="E8">
-        <v>2.3488525807857501</v>
+        <v>1.1423505902290301</v>
       </c>
       <c r="F8">
-        <v>2.2573738038539801</v>
+        <v>1.0354205906391101</v>
       </c>
       <c r="G8">
-        <v>2.2015236079692801</v>
+        <v>1.03215854465961</v>
       </c>
       <c r="H8">
-        <v>2.1965393364429402</v>
+        <v>1.0504649937152799</v>
       </c>
       <c r="I8">
-        <v>2.1926670074462802</v>
+        <v>1.1043696254491799</v>
       </c>
       <c r="J8">
-        <v>2.1880298495292601</v>
+        <v>1.1024294108152299</v>
       </c>
       <c r="K8">
-        <v>2.1684501767158499</v>
+        <v>1.0839870214462199</v>
       </c>
       <c r="L8">
-        <v>2.17634398937225</v>
+        <v>1.0775892078876399</v>
       </c>
       <c r="M8">
-        <v>2.1071691632270801</v>
+        <v>1.0612899214029301</v>
       </c>
       <c r="N8">
-        <v>2.07735979557037</v>
+        <v>1.0440317183732899</v>
       </c>
       <c r="O8">
-        <v>2.12588908672332</v>
+        <v>1.0615500897169099</v>
       </c>
       <c r="P8">
-        <v>2.0658591449260699</v>
+        <v>1.0472979605197901</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1"/>
@@ -9666,51 +9655,49 @@
       <c r="N10" s="1"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="A15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
     </row>
@@ -9725,8 +9712,7 @@
       <c r="C24" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A22:C24"/>
+  <mergeCells count="1">
     <mergeCell ref="A15:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9743,7 +9729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
@@ -9751,19 +9737,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>

<commit_message>
Completing the Difference Digest to work with StrataEstimators, and adding tests
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="IBF Decoding" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>10K</t>
   </si>
@@ -89,12 +89,21 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>PseudoRandom</t>
+  </si>
+  <si>
+    <t>HashFunctions</t>
+  </si>
+  <si>
+    <t>Pseudorandom</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,7 +153,12 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF008000"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -195,7 +209,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -255,8 +269,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,20 +347,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -320,6 +395,34 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -349,6 +452,34 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,10 +494,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -381,13 +512,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Percent</a:t>
+              <a:t>Percent Successfully Decoded vs. Set Difference w/ Pseudorandom Hash Functions</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Successfully Decoding vs. Set Difference</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -710,11 +836,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="2060985432"/>
-        <c:axId val="2060992472"/>
+        <c:axId val="2134022040"/>
+        <c:axId val="2133974344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2060985432"/>
+        <c:axId val="2134022040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,11 +857,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Set</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Difference</a:t>
+                  <a:t>Set Difference</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -747,7 +869,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060992472"/>
+        <c:crossAx val="2133974344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -755,7 +877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060992472"/>
+        <c:axId val="2133974344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +895,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percent Sucessfully Decoding</a:t>
+                  <a:t>Percent Sucessfully Decoded</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -785,7 +907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060985432"/>
+        <c:crossAx val="2134022040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -832,13 +954,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Percent</a:t>
+              <a:t>Percent Successfully Decoding vs. Set Difference</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Successfully Decoded vs Set Difference</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -848,29 +965,28 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>HashCount!$B$4</c:f>
+              <c:f>'IBF Decoding'!$M$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 Hash Functions</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>HashCount!$A$5:$A$15</c:f>
+              <c:f>'IBF Decoding'!$L$6:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -912,7 +1028,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HashCount!$B$5:$B$15</c:f>
+              <c:f>'IBF Decoding'!$M$6:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -920,60 +1036,57 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9954</c:v>
+                  <c:v>0.945999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.984099999999999</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.975533333333333</c:v>
+                  <c:v>0.963333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.957249999999997</c:v>
+                  <c:v>0.948</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.921439999999996</c:v>
+                  <c:v>0.928799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.84693333333333</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73905714285714</c:v>
+                  <c:v>0.755428571428571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5922</c:v>
+                  <c:v>0.329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.450977777777778</c:v>
+                  <c:v>0.162888888888888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.349179999999999</c:v>
+                  <c:v>0.0888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>HashCount!$C$4</c:f>
+              <c:f>'IBF Decoding'!$N$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3 Hash Functions</c:v>
+                  <c:v>1K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>HashCount!$A$5:$A$15</c:f>
+              <c:f>'IBF Decoding'!$L$6:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1015,7 +1128,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HashCount!$C$5:$C$15</c:f>
+              <c:f>'IBF Decoding'!$N$6:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1023,60 +1136,57 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9996</c:v>
+                  <c:v>0.959999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9994</c:v>
+                  <c:v>0.962</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.998933333333333</c:v>
+                  <c:v>0.944666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.997949999999999</c:v>
+                  <c:v>0.952</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.992759999999999</c:v>
+                  <c:v>0.9368</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.980566666666666</c:v>
+                  <c:v>0.919666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.886114285714285</c:v>
+                  <c:v>0.776285714285714</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.56495</c:v>
+                  <c:v>0.34525</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.294177777777778</c:v>
+                  <c:v>0.160222222222222</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.187199999999999</c:v>
+                  <c:v>0.0908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>HashCount!$D$4</c:f>
+              <c:f>'IBF Decoding'!$O$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4 Hash Functions</c:v>
+                  <c:v>10K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>HashCount!$A$5:$A$15</c:f>
+              <c:f>'IBF Decoding'!$L$6:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1118,7 +1228,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>HashCount!$D$5:$D$15</c:f>
+              <c:f>'IBF Decoding'!$O$6:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1126,245 +1236,55 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.957999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.952</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.947333333333332</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99985</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99848</c:v>
+                  <c:v>0.9272</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.978899999999999</c:v>
+                  <c:v>0.920666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.700857142857144</c:v>
+                  <c:v>0.782571428571427</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.259099999999999</c:v>
+                  <c:v>0.346749999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.125466666666667</c:v>
+                  <c:v>0.143555555555555</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0736800000000001</c:v>
+                  <c:v>0.0964</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:strRef>
-              <c:f>HashCount!$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5 Hash Functions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>100k</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:invertIfNegative val="0"/>
+          <c:val>
             <c:numRef>
-              <c:f>HashCount!$A$5:$A$15</c:f>
+              <c:f>'IBF Decoding'!$P$6:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>HashCount!$E$5:$E$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.9999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.99848</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.823699999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.262628571428572</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0993</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0512222222222226</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0274799999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>HashCount!$F$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>6 Hash Functions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>HashCount!$A$5:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>HashCount!$F$5:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.94768</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.392133333333334</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0985142857142865</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0435499999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0203999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0111399999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1374,13 +1294,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2043423624"/>
-        <c:axId val="2043429320"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="2136641320"/>
+        <c:axId val="2136805208"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2043423624"/>
+        <c:axId val="2136641320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,7 +1328,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043429320"/>
+        <c:crossAx val="2136805208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1417,7 +1336,672 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2043429320"/>
+        <c:axId val="2136805208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent Successfully Decoding</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2136641320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Successfully Decoded vs Set Difference w/ Pseudorandom Hash Functions</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$B$6:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9954</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.984099999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.975533333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.957249999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.921439999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84693333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73905714285714</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5922</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.450977777777778</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.349179999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$C$6:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.998933333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.997949999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.992759999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.980566666666666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.886114285714285</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56495</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.294177777777778</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.187199999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99848</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.978899999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.700857142857144</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.259099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.125466666666667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0736800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$E$6:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99848</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.823699999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.262628571428572</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0512222222222226</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0274799999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$F$6:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.392133333333334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0985142857142865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0435499999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0203999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0111399999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2060743384"/>
+        <c:axId val="2061020328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2060743384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Set Difference</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2061020328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2061020328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,7 +2036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043423624"/>
+        <c:crossAx val="2060743384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1474,7 +2058,676 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Percent Successfully Decoded vs Set Difference</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$I$6:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$J$6:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.977799999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.968599999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.959666666666661</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.943900000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.908919999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.841199999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.734485714285711</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59455</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.467933333333332</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.361499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$I$6:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$K$6:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.979399999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.973199999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.969666666666661</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.961350000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.958599999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.941166666666663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.878085714285711</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.357022222222222</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.211619999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$I$6:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$L$6:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.957599999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.950299999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.949533333333325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.943250000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.941039999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.921599999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.774171428571427</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3588</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.162311111111112</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0892</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$M$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$I$6:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$M$6:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.956399999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.948899999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.943333333333326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.936050000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.928359999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.858099999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.426657142857143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.140149999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0685111111111117</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0373999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HashCount!$N$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 Hash Functions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HashCount!$I$6:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HashCount!$N$6:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.956399999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.947799999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.943933333333326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.933950000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.916599999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.615466666666664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.159571428571429</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0636499999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0287333333333332</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0161599999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2135340728"/>
+        <c:axId val="2135115992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2135340728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Set Difference</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2135115992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2135115992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Successfully Decoded</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2135340728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1596,7 +2849,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1.00333333313465</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
@@ -1723,25 +2976,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.07529926896095</c:v>
+                  <c:v>1.09579387634992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.08812698423862</c:v>
+                  <c:v>1.03508435130119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.01024079322814</c:v>
+                  <c:v>1.05075427889823</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.01242186427116</c:v>
+                  <c:v>1.01050980657339</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.01861750781536</c:v>
+                  <c:v>1.01743366777896</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.04172211289405</c:v>
+                  <c:v>1.03164740473032</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>1.0116791421175</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0</c:v>
@@ -1750,7 +3003,7 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>1.00020833313465</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.0</c:v>
@@ -1850,49 +3103,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.0741450458765</c:v>
+                  <c:v>1.16440716266632</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.15862672030925</c:v>
+                  <c:v>1.12009355902671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0487130254507</c:v>
+                  <c:v>1.0815886837244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.07029258310794</c:v>
+                  <c:v>1.09207140266895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.02535218298435</c:v>
+                  <c:v>1.05936250150203</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.03294682800769</c:v>
+                  <c:v>1.04704635769128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.04675229787826</c:v>
+                  <c:v>1.04937990874052</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.03276591300964</c:v>
+                  <c:v>1.04738803327083</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.03747597336769</c:v>
+                  <c:v>1.04209456890821</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.02548971176147</c:v>
+                  <c:v>1.03155523836612</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.00244799256324</c:v>
+                  <c:v>1.02849391937255</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.00696150064468</c:v>
+                  <c:v>1.03343945533037</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.02781194150447</c:v>
+                  <c:v>1.03014725685119</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.01527112722396</c:v>
+                  <c:v>1.02874441444873</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.03154512643814</c:v>
+                  <c:v>1.03552802234888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1977,49 +3230,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.2318112373352</c:v>
+                  <c:v>1.18403708487749</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.15470606386661</c:v>
+                  <c:v>1.13467981994152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.17617998421192</c:v>
+                  <c:v>1.08610301971435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.14235059022903</c:v>
+                  <c:v>1.0896903181076</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.03542059063911</c:v>
+                  <c:v>1.07208668917417</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.03215854465961</c:v>
+                  <c:v>1.06753099501132</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.05046499371528</c:v>
+                  <c:v>1.05410169452428</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.10436962544918</c:v>
+                  <c:v>1.06538489878177</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.10242941081523</c:v>
+                  <c:v>1.086212823987</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.08398702144622</c:v>
+                  <c:v>1.06403309494256</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.07758920788764</c:v>
+                  <c:v>1.0622690758109</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.06128992140293</c:v>
+                  <c:v>1.06076446831226</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.04403171837329</c:v>
+                  <c:v>1.05096452742815</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.06155008971691</c:v>
+                  <c:v>1.05451318830251</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.04729796051979</c:v>
+                  <c:v>1.05790384799242</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2036,11 +3289,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2043480456"/>
-        <c:axId val="2043486264"/>
+        <c:axId val="2057170168"/>
+        <c:axId val="2135100232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2043480456"/>
+        <c:axId val="2057170168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,7 +3327,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043486264"/>
+        <c:crossAx val="2135100232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2082,7 +3335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2043486264"/>
+        <c:axId val="2135100232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2112,7 +3365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043480456"/>
+        <c:crossAx val="2057170168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2134,7 +3387,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2149,7 +3402,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -8194,11 +9446,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2043358472"/>
-        <c:axId val="2043454152"/>
+        <c:axId val="2056289832"/>
+        <c:axId val="2056292776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2043358472"/>
+        <c:axId val="2056289832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8208,7 +9460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043454152"/>
+        <c:crossAx val="2056292776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8216,7 +9468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2043454152"/>
+        <c:axId val="2056292776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8227,14 +9479,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2043358472"/>
+        <c:crossAx val="2056289832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8253,16 +9504,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8281,6 +9532,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8288,16 +9569,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8316,6 +9597,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8324,15 +9635,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8711,29 +10022,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:16">
+      <c r="A5" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" s="5">
         <v>100</v>
       </c>
@@ -8746,8 +10061,23 @@
       <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="L5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="5">
+        <v>100</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -8760,8 +10090,20 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -8774,8 +10116,20 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="L7" s="3">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>0.94599999999999895</v>
+      </c>
+      <c r="N7">
+        <v>0.95999999999999897</v>
+      </c>
+      <c r="O7">
+        <v>0.95799999999999896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="3">
         <v>10</v>
       </c>
@@ -8788,8 +10142,20 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="L8" s="3">
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>0.95</v>
+      </c>
+      <c r="N8">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="O8">
+        <v>0.95199999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="3">
         <v>15</v>
       </c>
@@ -8802,8 +10168,20 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="L9" s="3">
+        <v>15</v>
+      </c>
+      <c r="M9">
+        <v>0.96333333333333304</v>
+      </c>
+      <c r="N9">
+        <v>0.94466666666666599</v>
+      </c>
+      <c r="O9">
+        <v>0.94733333333333203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -8816,8 +10194,20 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="L10" s="3">
+        <v>20</v>
+      </c>
+      <c r="M10">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="N10">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="O10">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="3">
         <v>25</v>
       </c>
@@ -8830,8 +10220,20 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="L11" s="3">
+        <v>25</v>
+      </c>
+      <c r="M11">
+        <v>0.92879999999999896</v>
+      </c>
+      <c r="N11">
+        <v>0.93679999999999997</v>
+      </c>
+      <c r="O11">
+        <v>0.92720000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="3">
         <v>30</v>
       </c>
@@ -8844,8 +10246,20 @@
       <c r="D12">
         <v>0.961666666666666</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="L12" s="3">
+        <v>30</v>
+      </c>
+      <c r="M12">
+        <v>0.93</v>
+      </c>
+      <c r="N12">
+        <v>0.91966666666666597</v>
+      </c>
+      <c r="O12">
+        <v>0.92066666666666597</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="3">
         <v>35</v>
       </c>
@@ -8858,8 +10272,20 @@
       <c r="D13">
         <v>0.74057142857142799</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="L13" s="3">
+        <v>35</v>
+      </c>
+      <c r="M13">
+        <v>0.75542857142857101</v>
+      </c>
+      <c r="N13">
+        <v>0.77628571428571402</v>
+      </c>
+      <c r="O13">
+        <v>0.78257142857142703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="3">
         <v>40</v>
       </c>
@@ -8872,8 +10298,20 @@
       <c r="D14">
         <v>0.245749999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="L14" s="3">
+        <v>40</v>
+      </c>
+      <c r="M14">
+        <v>0.32999999999999902</v>
+      </c>
+      <c r="N14">
+        <v>0.34525</v>
+      </c>
+      <c r="O14">
+        <v>0.346749999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="3">
         <v>45</v>
       </c>
@@ -8886,8 +10324,20 @@
       <c r="D15">
         <v>0.13266666666666599</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="L15" s="3">
+        <v>45</v>
+      </c>
+      <c r="M15">
+        <v>0.162888888888888</v>
+      </c>
+      <c r="N15">
+        <v>0.16022222222222199</v>
+      </c>
+      <c r="O15">
+        <v>0.14355555555555499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="3">
         <v>50</v>
       </c>
@@ -8900,6 +10350,94 @@
       <c r="D16">
         <v>7.9600000000000004E-2</v>
       </c>
+      <c r="L16" s="3">
+        <v>50</v>
+      </c>
+      <c r="M16">
+        <v>8.8800000000000004E-2</v>
+      </c>
+      <c r="N16">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="O16">
+        <v>9.64E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="14" customHeight="1"/>
+    <row r="45" spans="1:13">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56"/>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57"/>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8915,18 +10453,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -8935,65 +10476,68 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
+      <c r="I5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="3">
         <v>0</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10">
-        <v>0.99539999999999995</v>
-      </c>
-      <c r="C6" s="10">
-        <v>0.99960000000000004</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
       <c r="E6" s="1">
@@ -9002,18 +10546,36 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3">
-        <v>10</v>
-      </c>
-      <c r="B7" s="10">
-        <v>0.98409999999999898</v>
-      </c>
-      <c r="C7" s="10">
-        <v>0.99939999999999996</v>
-      </c>
-      <c r="D7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.99539999999999995</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="1">
@@ -9022,18 +10584,36 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="I7" s="3">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.977799999999998</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.97939999999999805</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.95759999999999701</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.95639999999999703</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.95639999999999703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.97553333333333303</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.99893333333333301</v>
-      </c>
-      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.98409999999999898</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.99939999999999996</v>
+      </c>
+      <c r="D8" s="9">
         <v>1</v>
       </c>
       <c r="E8" s="1">
@@ -9042,296 +10622,425 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="I8" s="3">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.96859999999999602</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.97319999999999596</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.95029999999999504</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.94889999999999497</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.94779999999999498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
-        <v>0.95724999999999705</v>
+        <v>0.97553333333333303</v>
       </c>
       <c r="C9" s="1">
-        <v>0.997949999999999</v>
+        <v>0.99893333333333301</v>
       </c>
       <c r="D9" s="1">
-        <v>0.99985000000000002</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>0.99990000000000001</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="I9" s="3">
+        <v>15</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.95966666666666101</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.96966666666666101</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.94953333333332501</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.94333333333332603</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.94393333333332596</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.95724999999999705</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.997949999999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.99985000000000002</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.94390000000000096</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.96135000000000204</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.94325000000000303</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.93605000000000305</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.93395000000000294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="3">
         <v>25</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>0.92143999999999604</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>0.99275999999999898</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>0.99848000000000003</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>0.99848000000000003</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>0.94767999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3">
+      <c r="I11" s="3">
+        <v>25</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.90891999999999795</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.95859999999999901</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.94103999999999899</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.92835999999999796</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.91659999999999797</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="3">
         <v>30</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>0.84693333333332999</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>0.98056666666666603</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>0.97889999999999899</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>0.82369999999999899</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>0.392133333333334</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3">
+      <c r="I12" s="3">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.84119999999999695</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.94116666666666304</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.92159999999999498</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.85809999999999398</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.61546666666666405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="3">
         <v>35</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>0.73905714285713997</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>0.88611428571428497</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>0.70085714285714396</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>0.26262857142857199</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>9.8514285714286498E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3">
+      <c r="I13" s="3">
+        <v>35</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.73448571428571097</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.87808571428571103</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.77417142857142696</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.42665714285714301</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.159571428571429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="3">
         <v>40</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>0.59219999999999995</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>0.56494999999999995</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <v>0.259099999999999</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E14" s="1">
         <v>9.9299999999999999E-2</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F14" s="1">
         <v>4.35499999999997E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3">
+      <c r="I14" s="3">
+        <v>40</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.59455000000000002</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.35880000000000001</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.140149999999999</v>
+      </c>
+      <c r="N14" s="1">
+        <v>6.3649999999999707E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="3">
         <v>45</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>0.45097777777777798</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>0.29417777777777798</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>0.125466666666667</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>5.1222222222222599E-2</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <v>2.0399999999999901E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3">
+      <c r="I15" s="3">
+        <v>45</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.46793333333333198</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.35702222222222202</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.16231111111111199</v>
+      </c>
+      <c r="M15" s="1">
+        <v>6.8511111111111703E-2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>2.8733333333333201E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="3">
         <v>50</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>0.34917999999999899</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>0.18719999999999901</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <v>7.3680000000000107E-2</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>2.7479999999999699E-2</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <v>1.11399999999999E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="I16" s="3">
+        <v>50</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.36149999999999899</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.211619999999999</v>
+      </c>
+      <c r="L16" s="1">
+        <v>8.9200000000000002E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>3.7399999999999801E-2</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1.61599999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1"/>
+    <row r="25" spans="1:5">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:5">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+    <row r="27" spans="1:5">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+    <row r="28" spans="1:5">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
-      <c r="C31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
       <c r="C32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="C35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="C37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="C38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="C39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="C41" t="s">
-        <v>21</v>
-      </c>
+    <row r="49" spans="1:6">
+      <c r="A49" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A19:F23"/>
+    <mergeCell ref="A49:F53"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9346,15 +11055,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -9422,28 +11132,28 @@
       <c r="A5" s="3">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="14">
+        <v>1.0033333331346499</v>
+      </c>
+      <c r="C5" s="14">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="13">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="13">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5" s="13">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="13">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
+      <c r="I5" s="13">
         <v>1</v>
       </c>
       <c r="J5">
@@ -9472,35 +11182,35 @@
       <c r="A6" s="3">
         <v>100</v>
       </c>
-      <c r="B6">
-        <v>1.07529926896095</v>
-      </c>
-      <c r="C6">
-        <v>1.0881269842386201</v>
-      </c>
-      <c r="D6">
-        <v>1.0102407932281401</v>
-      </c>
-      <c r="E6">
-        <v>1.01242186427116</v>
-      </c>
-      <c r="F6">
-        <v>1.0186175078153601</v>
-      </c>
-      <c r="G6">
-        <v>1.0417221128940499</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
+      <c r="B6" s="14">
+        <v>1.09579387634992</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1.03508435130119</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1.05075427889823</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1.01050980657339</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1.0174336677789599</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1.0316474047303199</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1.0116791421175</v>
+      </c>
+      <c r="I6" s="13">
         <v>1</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>1.0002083331346501</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -9522,100 +11232,100 @@
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>1.0741450458765001</v>
-      </c>
-      <c r="C7">
-        <v>1.15862672030925</v>
-      </c>
-      <c r="D7">
-        <v>1.0487130254507</v>
-      </c>
-      <c r="E7">
-        <v>1.07029258310794</v>
-      </c>
-      <c r="F7">
-        <v>1.0253521829843499</v>
-      </c>
-      <c r="G7">
-        <v>1.0329468280076901</v>
-      </c>
-      <c r="H7">
-        <v>1.04675229787826</v>
-      </c>
-      <c r="I7">
-        <v>1.03276591300964</v>
+      <c r="B7" s="13">
+        <v>1.1644071626663199</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1.12009355902671</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1.0815886837244</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1.09207140266895</v>
+      </c>
+      <c r="F7" s="13">
+        <v>1.05936250150203</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1.0470463576912801</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1.04937990874052</v>
+      </c>
+      <c r="I7" s="13">
+        <v>1.0473880332708301</v>
       </c>
       <c r="J7">
-        <v>1.0374759733676899</v>
+        <v>1.04209456890821</v>
       </c>
       <c r="K7">
-        <v>1.0254897117614701</v>
+        <v>1.03155523836612</v>
       </c>
       <c r="L7">
-        <v>1.0024479925632399</v>
+        <v>1.02849391937255</v>
       </c>
       <c r="M7">
-        <v>1.0069615006446799</v>
+        <v>1.0334394553303701</v>
       </c>
       <c r="N7">
-        <v>1.02781194150447</v>
+        <v>1.03014725685119</v>
       </c>
       <c r="O7">
-        <v>1.0152711272239601</v>
+        <v>1.0287444144487301</v>
       </c>
       <c r="P7">
-        <v>1.0315451264381399</v>
+        <v>1.0355280223488801</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8">
-        <v>1.2318112373351999</v>
-      </c>
-      <c r="C8">
-        <v>1.15470606386661</v>
-      </c>
-      <c r="D8">
-        <v>1.17617998421192</v>
-      </c>
-      <c r="E8">
-        <v>1.1423505902290301</v>
-      </c>
-      <c r="F8">
-        <v>1.0354205906391101</v>
-      </c>
-      <c r="G8">
-        <v>1.03215854465961</v>
-      </c>
-      <c r="H8">
-        <v>1.0504649937152799</v>
-      </c>
-      <c r="I8">
-        <v>1.1043696254491799</v>
+      <c r="B8" s="13">
+        <v>1.1840370848774899</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1.13467981994152</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1.08610301971435</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1.0896903181076001</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1.07208668917417</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1.0675309950113201</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1.05410169452428</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1.06538489878177</v>
       </c>
       <c r="J8">
-        <v>1.1024294108152299</v>
+        <v>1.0862128239869999</v>
       </c>
       <c r="K8">
-        <v>1.0839870214462199</v>
+        <v>1.06403309494256</v>
       </c>
       <c r="L8">
-        <v>1.0775892078876399</v>
+        <v>1.0622690758108999</v>
       </c>
       <c r="M8">
-        <v>1.0612899214029301</v>
+        <v>1.0607644683122599</v>
       </c>
       <c r="N8">
-        <v>1.0440317183732899</v>
+        <v>1.0509645274281501</v>
       </c>
       <c r="O8">
-        <v>1.0615500897169099</v>
+        <v>1.0545131883025101</v>
       </c>
       <c r="P8">
-        <v>1.0472979605197901</v>
+        <v>1.0579038479924201</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -9654,68 +11364,90 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A15:F19"/>
+    <mergeCell ref="A14:F18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Updating hybrid, fixing key generation, and working on tests
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IBF Decoding" sheetId="1" r:id="rId1"/>
@@ -353,9 +353,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +360,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="115">
@@ -836,11 +836,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="2134022040"/>
-        <c:axId val="2133974344"/>
+        <c:axId val="2084551272"/>
+        <c:axId val="2080779848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134022040"/>
+        <c:axId val="2084551272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +869,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133974344"/>
+        <c:crossAx val="2080779848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -877,7 +877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133974344"/>
+        <c:axId val="2080779848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134022040"/>
+        <c:crossAx val="2084551272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1295,11 +1295,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2136641320"/>
-        <c:axId val="2136805208"/>
+        <c:axId val="2091681288"/>
+        <c:axId val="2059167176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2136641320"/>
+        <c:axId val="2091681288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1328,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136805208"/>
+        <c:crossAx val="2059167176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1336,7 +1336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136805208"/>
+        <c:axId val="2059167176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136641320"/>
+        <c:crossAx val="2091681288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1960,11 +1960,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2060743384"/>
-        <c:axId val="2061020328"/>
+        <c:axId val="2080785928"/>
+        <c:axId val="2080781400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2060743384"/>
+        <c:axId val="2080785928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,7 +1993,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2061020328"/>
+        <c:crossAx val="2080781400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2001,7 +2001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2061020328"/>
+        <c:axId val="2080781400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060743384"/>
+        <c:crossAx val="2080785928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2629,11 +2629,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2135340728"/>
-        <c:axId val="2135115992"/>
+        <c:axId val="-2146240040"/>
+        <c:axId val="2061280280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2135340728"/>
+        <c:axId val="-2146240040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2662,7 +2662,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135115992"/>
+        <c:crossAx val="2061280280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2670,7 +2670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135115992"/>
+        <c:axId val="2061280280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2705,7 +2705,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135340728"/>
+        <c:crossAx val="-2146240040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3289,11 +3289,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2057170168"/>
-        <c:axId val="2135100232"/>
+        <c:axId val="-2145767240"/>
+        <c:axId val="-2145761672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2057170168"/>
+        <c:axId val="-2145767240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3327,7 +3327,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135100232"/>
+        <c:crossAx val="-2145761672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3335,7 +3335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135100232"/>
+        <c:axId val="-2145761672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3365,7 +3365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057170168"/>
+        <c:crossAx val="-2145767240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3394,14 +3394,15 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3416,6 +3417,9 @@
           <c:tx>
             <c:v>Min-wise</c:v>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'Min Wise Hash Function'!$C$2:$C$1001</c:f>
@@ -9446,11 +9450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2056289832"/>
-        <c:axId val="2056292776"/>
+        <c:axId val="2084449576"/>
+        <c:axId val="2091639736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2056289832"/>
+        <c:axId val="2084449576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9460,7 +9464,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056292776"/>
+        <c:crossAx val="2091639736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9468,7 +9472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2056292776"/>
+        <c:axId val="2091639736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9479,13 +9483,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056289832"/>
+        <c:crossAx val="2084449576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10024,7 +10029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -10046,7 +10051,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="5">
@@ -10061,7 +10066,7 @@
       <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="M5" s="5">
@@ -10375,45 +10380,45 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51"/>
@@ -10441,7 +10446,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -10490,7 +10494,7 @@
       <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -10508,7 +10512,7 @@
       <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="5" t="s">
@@ -10997,53 +11001,52 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A49:F53"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11132,28 +11135,28 @@
       <c r="A5" s="3">
         <v>10</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>1.0033333331346499</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>1</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>1</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>1</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>1</v>
       </c>
       <c r="J5">
@@ -11182,28 +11185,28 @@
       <c r="A6" s="3">
         <v>100</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>1.09579387634992</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>1.03508435130119</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>1.05075427889823</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>1.01050980657339</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>1.0174336677789599</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>1.0316474047303199</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <v>1.0116791421175</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <v>1</v>
       </c>
       <c r="J6">
@@ -11232,28 +11235,28 @@
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>1.1644071626663199</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>1.12009355902671</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>1.0815886837244</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1.09207140266895</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>1.05936250150203</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>1.0470463576912801</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <v>1.04937990874052</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>1.0473880332708301</v>
       </c>
       <c r="J7">
@@ -11282,28 +11285,28 @@
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>1.1840370848774899</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>1.13467981994152</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>1.08610301971435</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>1.0896903181076001</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>1.07208668917417</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>1.0675309950113201</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>1.05410169452428</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <v>1.06538489878177</v>
       </c>
       <c r="J8">
@@ -11365,89 +11368,88 @@
       <c r="N10" s="1"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A14:F18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11461,8 +11463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updating results, running simulations for correction overhead for fixed size strata
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="IBF Decoding" sheetId="1" r:id="rId1"/>
@@ -209,8 +209,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -365,7 +377,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -423,6 +435,12 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -480,6 +498,12 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,19 +633,19 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.972333333333333</c:v>
+                  <c:v>0.987666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.702857142857143</c:v>
+                  <c:v>0.692285714285714</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2775</c:v>
+                  <c:v>0.2865</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.120888888888888</c:v>
+                  <c:v>0.127555555555555</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0727999999999999</c:v>
+                  <c:v>0.0724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,25 +727,25 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.998</c:v>
+                  <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.978333333333333</c:v>
+                  <c:v>0.994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.661142857142857</c:v>
+                  <c:v>0.688285714285714</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.246499999999999</c:v>
+                  <c:v>0.24375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.135999999999999</c:v>
+                  <c:v>0.143333333333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0738</c:v>
+                  <c:v>0.0733999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,19 +833,69 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.961666666666666</c:v>
+                  <c:v>0.973333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.740571428571428</c:v>
+                  <c:v>0.693714285714285</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.245749999999999</c:v>
+                  <c:v>0.255249999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.132666666666666</c:v>
+                  <c:v>0.124888888888888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0796</c:v>
+                  <c:v>0.0666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>100K</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'IBF Decoding'!$E$6:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.952</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.704571428571428</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24775</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.128666666666666</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -836,11 +910,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="2084551272"/>
-        <c:axId val="2080779848"/>
+        <c:axId val="-2146237384"/>
+        <c:axId val="2060857480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084551272"/>
+        <c:axId val="-2146237384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +943,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080779848"/>
+        <c:crossAx val="2060857480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -877,7 +951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080779848"/>
+        <c:axId val="2060857480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084551272"/>
+        <c:crossAx val="-2146237384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1036,34 +1110,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.967999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.962</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.945999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.963333333333333</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.948</c:v>
+                  <c:v>0.931</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.928799999999999</c:v>
+                  <c:v>0.950399999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.93</c:v>
+                  <c:v>0.920333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.755428571428571</c:v>
+                  <c:v>0.792285714285713</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.329999999999999</c:v>
+                  <c:v>0.33225</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.162888888888888</c:v>
+                  <c:v>0.153333333333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0888</c:v>
+                  <c:v>0.0978</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,34 +1210,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.959999999999999</c:v>
+                  <c:v>0.963999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.962</c:v>
+                  <c:v>0.946</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.944666666666666</c:v>
+                  <c:v>0.956666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.952</c:v>
+                  <c:v>0.9445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9368</c:v>
+                  <c:v>0.9312</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.919666666666666</c:v>
+                  <c:v>0.929</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.776285714285714</c:v>
+                  <c:v>0.763142857142856</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.34525</c:v>
+                  <c:v>0.314999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.160222222222222</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0908</c:v>
+                  <c:v>0.0856</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1236,34 +1310,34 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.957999999999999</c:v>
+                  <c:v>0.967999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.952</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.947333333333332</c:v>
+                  <c:v>0.956666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9375</c:v>
+                  <c:v>0.9465</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9272</c:v>
+                  <c:v>0.932799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.920666666666666</c:v>
+                  <c:v>0.934</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.782571428571427</c:v>
+                  <c:v>0.769714285714285</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.346749999999999</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.143555555555555</c:v>
+                  <c:v>0.16311111111111</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0964</c:v>
+                  <c:v>0.0942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1273,7 +1347,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>100k</c:v>
+            <c:v>100K</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -1282,6 +1356,39 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.953999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.943</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.955999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9445</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9308</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.904</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.750857142857142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34675</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.159333333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.098</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1295,11 +1402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2091681288"/>
-        <c:axId val="2059167176"/>
+        <c:axId val="2084344504"/>
+        <c:axId val="2060801448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091681288"/>
+        <c:axId val="2084344504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1435,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2059167176"/>
+        <c:crossAx val="2060801448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1336,7 +1443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2059167176"/>
+        <c:axId val="2060801448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,17 +1473,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091681288"/>
+        <c:crossAx val="2084344504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1426,7 +1529,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1960,11 +2062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2080785928"/>
-        <c:axId val="2080781400"/>
+        <c:axId val="2084520616"/>
+        <c:axId val="-2146104296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2080785928"/>
+        <c:axId val="2084520616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1986,14 +2088,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080781400"/>
+        <c:crossAx val="-2146104296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2001,7 +2102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080781400"/>
+        <c:axId val="-2146104296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2029,21 +2130,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080785928"/>
+        <c:crossAx val="2084520616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2095,7 +2194,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2629,11 +2727,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2146240040"/>
-        <c:axId val="2061280280"/>
+        <c:axId val="2084475336"/>
+        <c:axId val="2060880232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2146240040"/>
+        <c:axId val="2084475336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,14 +2753,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2061280280"/>
+        <c:crossAx val="2060880232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2670,7 +2767,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2061280280"/>
+        <c:axId val="2060880232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,21 +2795,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146240040"/>
+        <c:crossAx val="2084475336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2762,7 +2857,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3289,11 +3383,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145767240"/>
-        <c:axId val="-2145761672"/>
+        <c:axId val="2086607336"/>
+        <c:axId val="2137461448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145767240"/>
+        <c:axId val="2086607336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3320,14 +3414,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145761672"/>
+        <c:crossAx val="2137461448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3335,7 +3428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145761672"/>
+        <c:axId val="2137461448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,21 +3451,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145767240"/>
+        <c:crossAx val="2086607336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9450,11 +9541,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2084449576"/>
-        <c:axId val="2091639736"/>
+        <c:axId val="-2146212552"/>
+        <c:axId val="2059182776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2084449576"/>
+        <c:axId val="-2146212552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9464,7 +9555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091639736"/>
+        <c:crossAx val="2059182776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9472,7 +9563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091639736"/>
+        <c:axId val="2059182776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9483,7 +9574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084449576"/>
+        <c:crossAx val="-2146212552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10027,10 +10118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10086,25 +10177,31 @@
       <c r="A6" s="3">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="L6" s="3">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="10">
         <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
         <v>1</v>
       </c>
     </row>
@@ -10112,208 +10209,256 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="L7" s="3">
         <v>5</v>
       </c>
-      <c r="M7">
-        <v>0.94599999999999895</v>
+      <c r="M7" s="10">
+        <v>0.96799999999999897</v>
       </c>
       <c r="N7">
-        <v>0.95999999999999897</v>
+        <v>0.96399999999999897</v>
       </c>
       <c r="O7">
-        <v>0.95799999999999896</v>
+        <v>0.96799999999999897</v>
+      </c>
+      <c r="P7">
+        <v>0.95399999999999896</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="3">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="10">
         <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="L8" s="3">
         <v>10</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="10">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="N8">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="O8">
         <v>0.95</v>
       </c>
-      <c r="N8">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="O8">
-        <v>0.95199999999999996</v>
+      <c r="P8">
+        <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="3">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="10">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>1</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
       <c r="L9" s="3">
         <v>15</v>
       </c>
-      <c r="M9">
-        <v>0.96333333333333304</v>
+      <c r="M9" s="10">
+        <v>0.94599999999999895</v>
       </c>
       <c r="N9">
-        <v>0.94466666666666599</v>
+        <v>0.956666666666666</v>
       </c>
       <c r="O9">
-        <v>0.94733333333333203</v>
+        <v>0.956666666666666</v>
+      </c>
+      <c r="P9">
+        <v>0.95599999999999896</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="3">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>0.998</v>
+      <c r="C10" s="10">
+        <v>0.999</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="L10" s="3">
         <v>20</v>
       </c>
-      <c r="M10">
-        <v>0.94799999999999995</v>
+      <c r="M10" s="10">
+        <v>0.93100000000000005</v>
       </c>
       <c r="N10">
-        <v>0.95199999999999996</v>
+        <v>0.94450000000000001</v>
       </c>
       <c r="O10">
-        <v>0.9375</v>
+        <v>0.94650000000000001</v>
+      </c>
+      <c r="P10">
+        <v>0.94450000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="3">
         <v>25</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="10">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="L11" s="3">
         <v>25</v>
       </c>
-      <c r="M11">
-        <v>0.92879999999999896</v>
+      <c r="M11" s="10">
+        <v>0.95039999999999902</v>
       </c>
       <c r="N11">
-        <v>0.93679999999999997</v>
+        <v>0.93120000000000003</v>
       </c>
       <c r="O11">
-        <v>0.92720000000000002</v>
+        <v>0.93279999999999896</v>
+      </c>
+      <c r="P11">
+        <v>0.93079999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="3">
         <v>30</v>
       </c>
-      <c r="B12">
-        <v>0.97233333333333305</v>
-      </c>
-      <c r="C12">
-        <v>0.97833333333333306</v>
+      <c r="B12" s="10">
+        <v>0.98766666666666603</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.99399999999999999</v>
       </c>
       <c r="D12">
-        <v>0.961666666666666</v>
+        <v>0.97333333333333305</v>
+      </c>
+      <c r="E12">
+        <v>0.95199999999999996</v>
       </c>
       <c r="L12" s="3">
         <v>30</v>
       </c>
-      <c r="M12">
-        <v>0.93</v>
+      <c r="M12" s="10">
+        <v>0.920333333333333</v>
       </c>
       <c r="N12">
-        <v>0.91966666666666597</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="O12">
-        <v>0.92066666666666597</v>
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="P12">
+        <v>0.90400000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="3">
         <v>35</v>
       </c>
-      <c r="B13">
-        <v>0.70285714285714296</v>
-      </c>
-      <c r="C13">
-        <v>0.66114285714285703</v>
+      <c r="B13" s="10">
+        <v>0.69228571428571395</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.68828571428571395</v>
       </c>
       <c r="D13">
-        <v>0.74057142857142799</v>
+        <v>0.69371428571428495</v>
+      </c>
+      <c r="E13">
+        <v>0.70457142857142796</v>
       </c>
       <c r="L13" s="3">
         <v>35</v>
       </c>
-      <c r="M13">
-        <v>0.75542857142857101</v>
+      <c r="M13" s="10">
+        <v>0.79228571428571304</v>
       </c>
       <c r="N13">
-        <v>0.77628571428571402</v>
+        <v>0.76314285714285601</v>
       </c>
       <c r="O13">
-        <v>0.78257142857142703</v>
+        <v>0.76971428571428502</v>
+      </c>
+      <c r="P13">
+        <v>0.750857142857142</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="3">
         <v>40</v>
       </c>
-      <c r="B14">
-        <v>0.27750000000000002</v>
-      </c>
-      <c r="C14">
-        <v>0.246499999999999</v>
+      <c r="B14" s="10">
+        <v>0.28649999999999998</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.24374999999999999</v>
       </c>
       <c r="D14">
-        <v>0.245749999999999</v>
+        <v>0.25524999999999898</v>
+      </c>
+      <c r="E14">
+        <v>0.24775</v>
       </c>
       <c r="L14" s="3">
         <v>40</v>
       </c>
-      <c r="M14">
-        <v>0.32999999999999902</v>
+      <c r="M14" s="10">
+        <v>0.33224999999999999</v>
       </c>
       <c r="N14">
-        <v>0.34525</v>
+        <v>0.314999999999999</v>
       </c>
       <c r="O14">
-        <v>0.346749999999999</v>
+        <v>0.34</v>
+      </c>
+      <c r="P14">
+        <v>0.34675</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -10321,25 +10466,31 @@
         <v>45</v>
       </c>
       <c r="B15">
-        <v>0.120888888888888</v>
+        <v>0.12755555555555501</v>
       </c>
       <c r="C15">
-        <v>0.13599999999999901</v>
+        <v>0.14333333333333301</v>
       </c>
       <c r="D15">
-        <v>0.13266666666666599</v>
+        <v>0.12488888888888799</v>
+      </c>
+      <c r="E15">
+        <v>0.12866666666666601</v>
       </c>
       <c r="L15" s="3">
         <v>45</v>
       </c>
-      <c r="M15">
-        <v>0.162888888888888</v>
+      <c r="M15" s="10">
+        <v>0.15333333333333299</v>
       </c>
       <c r="N15">
         <v>0.16022222222222199</v>
       </c>
       <c r="O15">
-        <v>0.14355555555555499</v>
+        <v>0.16311111111111001</v>
+      </c>
+      <c r="P15">
+        <v>0.15933333333333299</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -10347,105 +10498,43 @@
         <v>50</v>
       </c>
       <c r="B16">
-        <v>7.2799999999999906E-2</v>
+        <v>7.2400000000000006E-2</v>
       </c>
       <c r="C16">
-        <v>7.3800000000000004E-2</v>
+        <v>7.3399999999999896E-2</v>
       </c>
       <c r="D16">
-        <v>7.9600000000000004E-2</v>
+        <v>6.6600000000000006E-2</v>
+      </c>
+      <c r="E16">
+        <v>6.9199999999999998E-2</v>
       </c>
       <c r="L16" s="3">
         <v>50</v>
       </c>
       <c r="M16">
-        <v>8.8800000000000004E-2</v>
+        <v>9.7799999999999998E-2</v>
       </c>
       <c r="N16">
-        <v>9.0800000000000006E-2</v>
+        <v>8.5599999999999996E-2</v>
       </c>
       <c r="O16">
-        <v>9.64E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="14" customHeight="1"/>
-    <row r="45" spans="1:13">
+        <v>9.4200000000000006E-2</v>
+      </c>
+      <c r="P16">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="14" customHeight="1"/>
+    <row r="45" spans="1:1">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:1">
       <c r="A46"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56"/>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11463,8 +11552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Strata estimator working with cutoff
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -910,11 +910,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="-2146237384"/>
-        <c:axId val="2060857480"/>
+        <c:axId val="-2146000024"/>
+        <c:axId val="2086824120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146237384"/>
+        <c:axId val="-2146000024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +943,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060857480"/>
+        <c:crossAx val="2086824120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -951,7 +951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060857480"/>
+        <c:axId val="2086824120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146237384"/>
+        <c:crossAx val="-2146000024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1402,11 +1402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2084344504"/>
-        <c:axId val="2060801448"/>
+        <c:axId val="-2146434872"/>
+        <c:axId val="2091954872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084344504"/>
+        <c:axId val="-2146434872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1435,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060801448"/>
+        <c:crossAx val="2091954872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060801448"/>
+        <c:axId val="2091954872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084344504"/>
+        <c:crossAx val="-2146434872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1529,6 +1529,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2062,11 +2063,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2084520616"/>
-        <c:axId val="-2146104296"/>
+        <c:axId val="2085756280"/>
+        <c:axId val="2086636632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2084520616"/>
+        <c:axId val="2085756280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,13 +2089,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146104296"/>
+        <c:crossAx val="2086636632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2102,7 +2104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146104296"/>
+        <c:axId val="2086636632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2130,19 +2132,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084520616"/>
+        <c:crossAx val="2085756280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2194,6 +2198,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2727,11 +2732,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2084475336"/>
-        <c:axId val="2060880232"/>
+        <c:axId val="2137614760"/>
+        <c:axId val="2086390872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2084475336"/>
+        <c:axId val="2137614760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2753,13 +2758,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2060880232"/>
+        <c:crossAx val="2086390872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2767,7 +2773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2060880232"/>
+        <c:axId val="2086390872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,19 +2801,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084475336"/>
+        <c:crossAx val="2137614760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2857,6 +2865,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3383,11 +3392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2086607336"/>
-        <c:axId val="2137461448"/>
+        <c:axId val="2086842488"/>
+        <c:axId val="2092007640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2086607336"/>
+        <c:axId val="2086842488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3414,13 +3423,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137461448"/>
+        <c:crossAx val="2092007640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3428,7 +3438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137461448"/>
+        <c:axId val="2092007640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3451,19 +3461,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086607336"/>
+        <c:crossAx val="2086842488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9541,11 +9553,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2146212552"/>
-        <c:axId val="2059182776"/>
+        <c:axId val="-2145907800"/>
+        <c:axId val="2086893512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2146212552"/>
+        <c:axId val="-2145907800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9555,7 +9567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2059182776"/>
+        <c:crossAx val="2086893512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9563,7 +9575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2059182776"/>
+        <c:axId val="2086893512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9574,7 +9586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146212552"/>
+        <c:crossAx val="-2145907800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10120,8 +10132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10534,7 +10546,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11150,7 +11161,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11552,7 +11563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>

</xml_diff>